<commit_message>
Update SCD0026-001 until SCD0026-017 Fix
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0026-001 - View agenda pada Mobile.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0026-001 - View agenda pada Mobile.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB41F802-9C52-4CBA-870B-7C65F69E2D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB406CC-8997-4288-8BA5-FE8C73F42016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SCD0338" sheetId="2" r:id="rId1"/>
+    <sheet name="SCD0026" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,9 +92,6 @@
     <t>TEXT5</t>
   </si>
   <si>
-    <t>SCD0338-001</t>
-  </si>
-  <si>
     <t>View agenda pada Mobile</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Test Daily Activity 5</t>
+  </si>
+  <si>
+    <t>SCD0026-001</t>
   </si>
 </sst>
 </file>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +622,7 @@
         <v>19</v>
       </c>
       <c r="Q1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="172.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -630,16 +630,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="F2" s="10">
         <v>43988</v>
@@ -657,26 +657,26 @@
         <v>17</v>
       </c>
       <c r="K2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="N2" s="15" t="str">
         <f ca="1">TEXT(TODAY(),"dd-mmm-yyyy")</f>
-        <v>07-Nov-2022</v>
+        <v>08-Nov-2022</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
@@ -686,16 +686,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="F3" s="10">
         <v>103258</v>
@@ -713,26 +713,26 @@
         <v>17</v>
       </c>
       <c r="K3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="N3" s="15" t="str">
         <f ca="1">TEXT(TODAY(),"dd-mmm-yyyy")</f>
-        <v>07-Nov-2022</v>
+        <v>08-Nov-2022</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>